<commit_message>
Added JS price countera to all items. Adjusted total price. Fixed several id names.
</commit_message>
<xml_diff>
--- a/app/static/texts/ItemDatabase.xlsx
+++ b/app/static/texts/ItemDatabase.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE95F17-E43E-40C4-BE3B-AAC57F01955C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74496F5D-5873-45EA-9756-4FD7CE694428}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Item Type</t>
   </si>
@@ -58,15 +64,6 @@
     <t>Jumpsuits 1 month</t>
   </si>
   <si>
-    <t>Jacket</t>
-  </si>
-  <si>
-    <t>Hat</t>
-  </si>
-  <si>
-    <t>Soft shoes</t>
-  </si>
-  <si>
     <t>Infant bath tub</t>
   </si>
   <si>
@@ -163,16 +160,25 @@
     <t>Diaper pail</t>
   </si>
   <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>Swing</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Total price</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -182,18 +188,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -208,10 +208,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,416 +491,689 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>199.99</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <f>B2*C2</f>
+        <v>199.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>179.99</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D44" si="0">B3*C3</f>
+        <v>179.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>46.99</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>46.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>13.47</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>13.47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>12.97</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>12.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>36.99</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>36.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>12</v>
       </c>
-      <c r="C8" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>8</v>
       </c>
-      <c r="C9" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>12</v>
       </c>
-      <c r="C10" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>24.99</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>24.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>6.97</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>6.97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>25.99</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>25.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
-        <v>24.99</v>
-      </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
-        <v>6.97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
-        <v>25.99</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>249.96</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>249.96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
-        <v>6.99</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>53.38</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>53.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>30.99</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>61.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20">
-        <v>249.96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>20.99</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>20.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21">
-        <v>53.38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>21.99</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>21.99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22">
-        <v>30.99</v>
-      </c>
-      <c r="C22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23">
-        <v>20.99</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>3.78</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1">
+        <v>141.1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>141.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B24">
-        <v>21.99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" s="1">
+        <v>48.99</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>48.99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B25">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B26">
-        <v>3.78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27">
-        <v>141.1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28">
-        <v>48.99</v>
-      </c>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>10.039999999999999</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>10.039999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>15.99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>28.98</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>28.98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>19.989999999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B32">
-        <v>10.039999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33">
-        <v>28.98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>19.989999999999998</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B35">
-        <v>6.99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>10.95</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B36">
-        <v>9.99</v>
-      </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>22.99</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>22.99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B37">
-        <v>15.99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B38">
-        <v>10.95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>11.48</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>11.48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39">
-        <v>22.99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>39.76</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>39.76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B40">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>46.7</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>46.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B41">
-        <v>11.48</v>
-      </c>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>14.99</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B42">
-        <v>39.76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B43">
-        <v>46.7</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5199999999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B44">
-        <v>14.99</v>
-      </c>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="0"/>
+        <v>79.989999999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>2.2400000000000002</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>4.5199999999999996</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>79.989999999999995</v>
+        <v>47</v>
+      </c>
+      <c r="D45" s="1">
+        <f>SUM(D2:D44)</f>
+        <v>1620.0700000000002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>